<commit_message>
Added more users and time slots
</commit_message>
<xml_diff>
--- a/Accounts.xlsx
+++ b/Accounts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ScheduleMeWorkspace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ScheduleMeWorkspaceData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED993B9D-4B1C-4EBB-A7AB-939945B797A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549E9DC7-7F76-4D7A-81F6-0A2093B09F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72B11D14-9F55-4053-B446-41510EABE26B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{72B11D14-9F55-4053-B446-41510EABE26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="64">
   <si>
     <t>Mr</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>EMHC  Reader2</t>
+  </si>
+  <si>
+    <t>Beata</t>
+  </si>
+  <si>
+    <t>bdalecka@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -591,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9888F6-CB3A-4AEC-97FB-01C2A5FDD384}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,13 +1293,41 @@
       <c r="I25" s="2"/>
       <c r="J25" s="3"/>
     </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="3">
+        <v>35953</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="3"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E24:E25 E1:E16" xr:uid="{791B9466-C7A2-4D25-8A34-F6908D93841E}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E24:E26 E1:E16" xr:uid="{791B9466-C7A2-4D25-8A34-F6908D93841E}">
       <formula1>10</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J25" xr:uid="{210908B5-77AD-4D06-B456-E11B9ED84CEC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J26" xr:uid="{210908B5-77AD-4D06-B456-E11B9ED84CEC}">
       <formula1>Dates</formula1>
     </dataValidation>
   </dataValidations>
@@ -1354,8 +1388,10 @@
     <hyperlink ref="G17" r:id="rId54" xr:uid="{9FD5D1B5-01ED-47A4-8522-778CD05B66A4}"/>
     <hyperlink ref="D22" r:id="rId55" xr:uid="{3B0A713F-83A7-4CAF-A4F8-4E49F2DA8190}"/>
     <hyperlink ref="G22" r:id="rId56" xr:uid="{85F150D6-3516-4046-B961-FC1B4506CC4A}"/>
+    <hyperlink ref="D26" r:id="rId57" xr:uid="{49915CE3-3B9B-42CD-928F-FC7ED870339B}"/>
+    <hyperlink ref="G26" r:id="rId58" xr:uid="{DA36F0D9-284E-43CD-9A4C-FAF35BA636FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId57"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId59"/>
 </worksheet>
 </file>
</xml_diff>